<commit_message>
Learning more about VBA
</commit_message>
<xml_diff>
--- a/VBA/theFirstMacro.xlsx
+++ b/VBA/theFirstMacro.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B65D5477-9DC4-4BED-9726-D2E3981C00BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73338E42-1827-44F0-A530-68375FAE3FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{464B64E1-5688-45A1-8EE8-816F86F9099C}"/>
+    <workbookView xWindow="-4800" yWindow="-15870" windowWidth="25440" windowHeight="15990" activeTab="3" xr2:uid="{464B64E1-5688-45A1-8EE8-816F86F9099C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +35,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t>Yes!!!!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,11 +417,11 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <f ca="1">NOW()</f>
-        <v>45336.961835069444</v>
+        <v>45345.463421412038</v>
       </c>
       <c r="C1" s="1">
         <f ca="1">NOW()</f>
-        <v>45336.961835069444</v>
+        <v>45345.463421412038</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -433,25 +443,83 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <f ca="1">NOW()</f>
-        <v>45336.961835069444</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5968FD84-71BE-467C-88B2-24A3959E490A}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q33" sqref="Q33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A8A2E4-F20E-4652-B1DD-B14618572AF9}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>